<commit_message>
New test with more dimensions
</commit_message>
<xml_diff>
--- a/results/planning/two_node_analysis.xlsx
+++ b/results/planning/two_node_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmailcarletonca-my.sharepoint.com/personal/luislopezdiaz_cmail_carleton_ca/Documents/00 PhD Thesis/code/GridOpt.jl/results/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="738" documentId="8_{15012C9A-1165-432B-9B86-14D9CC3D97E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E82ECC36-EC01-4500-A700-38DDEF4CEFFE}"/>
+  <xr:revisionPtr revIDLastSave="754" documentId="8_{15012C9A-1165-432B-9B86-14D9CC3D97E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2619983B-4208-4A82-8E71-44770F6BECF4}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="1" xr2:uid="{2A8ECC8D-33BE-457A-B507-D9BBA4748D0E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2A8ECC8D-33BE-457A-B507-D9BBA4748D0E}"/>
   </bookViews>
   <sheets>
     <sheet name="two_nodes" sheetId="2" r:id="rId1"/>
@@ -299,6 +299,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,22 +323,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -669,39 +669,39 @@
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26171875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.41796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19" t="s">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
@@ -718,7 +718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="Q2">
         <v>150</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="S2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="T2" s="6" t="s">
@@ -795,7 +795,7 @@
         <v>246.5</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -847,7 +847,7 @@
       <c r="Q3">
         <v>2</v>
       </c>
-      <c r="S3" s="23"/>
+      <c r="S3" s="17"/>
       <c r="T3" t="s">
         <v>23</v>
       </c>
@@ -868,7 +868,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="Q4" s="2">
         <v>42.089999999999897</v>
       </c>
-      <c r="S4" s="23"/>
+      <c r="S4" s="17"/>
       <c r="T4" t="s">
         <v>24</v>
       </c>
@@ -940,7 +940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -992,7 +992,7 @@
       <c r="Q5" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="23"/>
+      <c r="S5" s="17"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
         <v>29</v>
@@ -1010,7 +1010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1062,7 +1062,7 @@
       <c r="Q6">
         <v>0</v>
       </c>
-      <c r="S6" s="23"/>
+      <c r="S6" s="17"/>
       <c r="T6" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1137,7 +1137,7 @@
       <c r="Q7">
         <v>400</v>
       </c>
-      <c r="S7" s="23"/>
+      <c r="S7" s="17"/>
       <c r="T7" t="s">
         <v>22</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>167.5</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="Q8">
         <v>550</v>
       </c>
-      <c r="S8" s="23"/>
+      <c r="S8" s="17"/>
       <c r="T8" t="s">
         <v>25</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="S9" s="24"/>
+      <c r="S9" s="18"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3" t="s">
         <v>29</v>
@@ -1302,7 +1302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="Q10">
         <v>2</v>
       </c>
-      <c r="S10" s="22" t="s">
+      <c r="S10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="T10" s="6" t="s">
@@ -1379,7 +1379,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="Q11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S11" s="23"/>
+      <c r="S11" s="17"/>
       <c r="T11" t="s">
         <v>23</v>
       </c>
@@ -1451,8 +1451,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="S12" s="23"/>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S12" s="17"/>
       <c r="T12" t="s">
         <v>26</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -1503,7 +1503,7 @@
       <c r="K13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S13" s="23"/>
+      <c r="S13" s="17"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1" t="s">
         <v>29</v>
@@ -1521,8 +1521,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B14">
@@ -1555,7 +1555,7 @@
       <c r="K14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S14" s="23"/>
+      <c r="S14" s="17"/>
       <c r="T14" t="s">
         <v>21</v>
       </c>
@@ -1578,8 +1578,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="19"/>
+    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
       <c r="B15">
         <v>167.5</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="K15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S15" s="23"/>
+      <c r="S15" s="17"/>
       <c r="T15" t="s">
         <v>22</v>
       </c>
@@ -1633,8 +1633,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="19"/>
+    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
       <c r="B16">
         <v>0</v>
       </c>
@@ -1665,7 +1665,7 @@
       <c r="K16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S16" s="23"/>
+      <c r="S16" s="17"/>
       <c r="T16" t="s">
         <v>27</v>
       </c>
@@ -1685,8 +1685,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="19"/>
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
       <c r="B17">
         <v>200</v>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="K17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S17" s="24"/>
+      <c r="S17" s="18"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3" t="s">
         <v>29</v>
@@ -1735,8 +1735,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B18">
@@ -1769,16 +1769,16 @@
       <c r="K18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S18" s="18" t="s">
+      <c r="S18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-    </row>
-    <row r="19" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="21"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
       <c r="B19">
         <v>200</v>
       </c>
@@ -1810,8 +1810,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="21"/>
+    <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="24"/>
       <c r="B20">
         <v>0</v>
       </c>
@@ -1857,8 +1857,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="19"/>
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
       <c r="B21">
         <v>200</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="K21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="T21" s="15" t="s">
+      <c r="T21" s="19" t="s">
         <v>32</v>
       </c>
       <c r="U21" t="s">
@@ -1908,8 +1908,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="19" t="s">
+    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -1942,7 +1942,7 @@
       <c r="K22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="16"/>
+      <c r="T22" s="20"/>
       <c r="U22" s="3" t="s">
         <v>12</v>
       </c>
@@ -1959,8 +1959,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="19"/>
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
       <c r="B23">
         <v>67.5</v>
       </c>
@@ -1991,10 +1991,10 @@
       <c r="K23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T23" s="17" t="s">
+      <c r="T23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="U23" s="17"/>
+      <c r="U23" s="21"/>
       <c r="V23" s="14">
         <v>300</v>
       </c>
@@ -2008,8 +2008,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="19"/>
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
       <c r="B24">
         <v>0</v>
       </c>
@@ -2042,8 +2042,8 @@
       </c>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="19"/>
+    <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
       <c r="B25">
         <v>150</v>
       </c>
@@ -2075,8 +2075,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="19" t="s">
+    <row r="26" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B26">
@@ -2111,8 +2111,8 @@
       </c>
       <c r="T26" s="4"/>
     </row>
-    <row r="27" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A27" s="19"/>
+    <row r="27" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
       <c r="B27">
         <v>167.5</v>
       </c>
@@ -2144,8 +2144,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="19"/>
+    <row r="28" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
       <c r="B28">
         <v>0</v>
       </c>
@@ -2177,8 +2177,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A29" s="19"/>
+    <row r="29" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
       <c r="B29">
         <v>150</v>
       </c>
@@ -2212,6 +2212,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="S18:W18"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="S10:S17"/>
     <mergeCell ref="S2:S9"/>
@@ -2219,12 +2225,6 @@
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="S18:W18"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2232,39 +2232,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9E9B71-9EB2-402B-A29F-5B0BB42EA6E4}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.62890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2281,16 +2278,28 @@
         <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>20</v>
+      </c>
+      <c r="S2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2307,16 +2316,19 @@
         <v>15</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0.27</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>1.56</v>
       </c>
       <c r="H3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>1.64</v>
+      </c>
+      <c r="I3">
+        <v>12.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2333,16 +2345,19 @@
         <v>32</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>3.31</v>
       </c>
       <c r="H4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>3.57</v>
+      </c>
+      <c r="I4">
+        <v>8.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -2359,19 +2374,16 @@
         <v>64</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3.26</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>19.32</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>43.21</v>
       </c>
       <c r="I5">
-        <v>3.26</v>
-      </c>
-      <c r="J5">
-        <v>19.32</v>
+        <v>333.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>